<commit_message>
Servo PWM pullups corrected, battery voltage divider adjusted
schematic layout improved, signal names unified
</commit_message>
<xml_diff>
--- a/teensy/teensy_3.6_pin_mapping.xlsx
+++ b/teensy/teensy_3.6_pin_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ts/src/ctbot/ct-bot-hw/teensy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB6FE55-8C50-B743-A428-616F126EF5DB}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF8EEA9-8D11-354D-A961-72728FEE2E2B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="40920" windowHeight="29060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="201">
   <si>
     <t>Pin</t>
   </si>
@@ -99,9 +99,6 @@
     <t>A10</t>
   </si>
   <si>
-    <t>PWM0</t>
-  </si>
-  <si>
     <t>Servo 1</t>
   </si>
   <si>
@@ -615,9 +612,6 @@
     <t>MAUS_D_3V3</t>
   </si>
   <si>
-    <t>This work is licensed under the Creative Commons Attribution-ShareAlike 4.0 International License. To view a copy of this license, visit http://creativecommons.org/licenses/by-sa/4.0/ or send a letter to Creative Commons, PO Box 1866, Mountain View, CA 94042, USA.</t>
-  </si>
-  <si>
     <t>D+</t>
   </si>
   <si>
@@ -628,6 +622,15 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>This work is licensed under the Creative Commons Attribution-ShareAlike 4.0 International License. To view a copy of this license, visit http://creativecommons.org/licenses/by-sa/4.0</t>
+  </si>
+  <si>
+    <t>PWM1</t>
+  </si>
+  <si>
+    <t>BAT_IN_FB</t>
   </si>
 </sst>
 </file>
@@ -1046,15 +1049,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>244928</xdr:colOff>
+      <xdr:colOff>312615</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>117928</xdr:rowOff>
+      <xdr:rowOff>30007</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>141111</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>162187</xdr:rowOff>
+      <xdr:colOff>283309</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>85902</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1077,13 +1080,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="30801" t="5507" r="345" b="4854"/>
+        <a:srcRect l="32720" t="5507" r="230" b="4854"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9268984" y="5028595"/>
-          <a:ext cx="5674683" cy="5364148"/>
+          <a:off x="9202615" y="4953699"/>
+          <a:ext cx="5783386" cy="5595049"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1095,7 +1098,7 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>952499</xdr:colOff>
+      <xdr:colOff>634999</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>154214</xdr:rowOff>
     </xdr:from>
@@ -1131,8 +1134,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8182428" y="154214"/>
-          <a:ext cx="7712018" cy="4699000"/>
+          <a:off x="8059614" y="154214"/>
+          <a:ext cx="7755980" cy="4832978"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1191,6 +1194,65 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>502278</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>102584</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5090653" cy="233205"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Textfeld 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D8AF4AC-71AA-9742-B813-0807FB0B26C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="9392278" y="10565430"/>
+          <a:ext cx="5090653" cy="233205"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="900"/>
+            <a:t>Sources: https://www.pjrc.com/teensy/card9a_rev1.pdf; https://www.pjrc.com/teensy/card9b_rev1.pdf</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1463,17 +1525,18 @@
   <dimension ref="A1:L76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="13" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="6.6640625" customWidth="1"/>
+    <col min="9" max="9" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.33203125" customWidth="1"/>
   </cols>
@@ -1489,31 +1552,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E1" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="G1" s="62" t="s">
         <v>150</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="H1" s="62" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="62" t="s">
-        <v>152</v>
-      </c>
       <c r="I1" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" s="63" t="s">
-        <v>56</v>
-      </c>
       <c r="L1" s="63" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1521,13 +1584,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="84"/>
       <c r="F2" s="51"/>
@@ -1537,7 +1600,7 @@
       </c>
       <c r="I2" s="55"/>
       <c r="J2" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K2" s="55"/>
       <c r="L2" s="55"/>
@@ -1547,13 +1610,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="45" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="85"/>
       <c r="F3" s="52"/>
@@ -1563,7 +1626,7 @@
       </c>
       <c r="I3" s="56"/>
       <c r="J3" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K3" s="56"/>
       <c r="L3" s="56"/>
@@ -1573,22 +1636,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E4" s="76" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F4" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H4" s="50" t="s">
         <v>9</v>
@@ -1596,10 +1659,10 @@
       <c r="I4" s="57"/>
       <c r="J4" s="57"/>
       <c r="K4" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L4" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -1607,29 +1670,29 @@
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E5" s="71" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="22" t="s">
         <v>4</v>
       </c>
       <c r="G5" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="22" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="55"/>
       <c r="J5" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K5" s="55"/>
       <c r="L5" s="55"/>
@@ -1639,29 +1702,29 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="45" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" s="80" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="47" t="s">
         <v>5</v>
       </c>
       <c r="G6" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H6" s="45" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="56"/>
       <c r="J6" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K6" s="56"/>
       <c r="L6" s="56"/>
@@ -1671,28 +1734,28 @@
         <v>5</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C7" s="46" t="s">
+        <v>199</v>
+      </c>
+      <c r="D7" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="46" t="s">
-        <v>24</v>
-      </c>
       <c r="E7" s="79" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H7" s="46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I7" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J7" s="55"/>
       <c r="K7" s="55"/>
@@ -1703,33 +1766,33 @@
         <v>6</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="47" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="80" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G8" s="47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H8" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I8" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J8" s="56"/>
       <c r="K8" s="56"/>
       <c r="L8" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1737,33 +1800,33 @@
         <v>7</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E9" s="79" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I9" s="55"/>
       <c r="J9" s="55"/>
       <c r="K9" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L9" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -1771,33 +1834,33 @@
         <v>8</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E10" s="81" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F10" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H10" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I10" s="58"/>
       <c r="J10" s="58"/>
       <c r="K10" s="58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L10" s="58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -1805,27 +1868,27 @@
         <v>9</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E11" s="79"/>
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
       <c r="H11" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I11" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J11" s="55"/>
       <c r="K11" s="55"/>
       <c r="L11" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1833,27 +1896,27 @@
         <v>10</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E12" s="81"/>
       <c r="F12" s="48"/>
       <c r="G12" s="48"/>
       <c r="H12" s="49" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I12" s="58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J12" s="58"/>
       <c r="K12" s="58"/>
       <c r="L12" s="58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1864,24 +1927,24 @@
         <v>6</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="79"/>
       <c r="F13" s="46"/>
       <c r="G13" s="46"/>
       <c r="H13" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I13" s="55"/>
       <c r="J13" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K13" s="55"/>
       <c r="L13" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1892,24 +1955,24 @@
         <v>7</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D14" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E14" s="80"/>
       <c r="F14" s="47"/>
       <c r="G14" s="47"/>
       <c r="H14" s="45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I14" s="56"/>
       <c r="J14" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K14" s="56"/>
       <c r="L14" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1920,7 +1983,7 @@
         <v>8</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>8</v>
@@ -1929,11 +1992,11 @@
       <c r="F15" s="50"/>
       <c r="G15" s="50"/>
       <c r="H15" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I15" s="57"/>
       <c r="J15" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K15" s="57"/>
       <c r="L15" s="10"/>
@@ -1943,27 +2006,27 @@
         <v>14</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C16" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>112</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>113</v>
       </c>
       <c r="E16" s="79"/>
       <c r="F16" s="46"/>
       <c r="G16" s="46"/>
       <c r="H16" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I16" s="55"/>
       <c r="J16" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K16" s="55"/>
       <c r="L16" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1971,27 +2034,27 @@
         <v>15</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D17" s="45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E17" s="80"/>
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
       <c r="H17" s="45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I17" s="56"/>
       <c r="J17" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K17" s="56"/>
       <c r="L17" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1999,28 +2062,28 @@
         <v>16</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="79" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G18" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H18" s="46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I18" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J18" s="55"/>
       <c r="K18" s="55"/>
@@ -2031,28 +2094,28 @@
         <v>17</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="69" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F19" s="69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G19" s="69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H19" s="79" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I19" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J19" s="55"/>
       <c r="K19" s="55"/>
@@ -2063,28 +2126,28 @@
         <v>18</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F20" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G20" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H20" s="46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I20" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J20" s="55"/>
       <c r="K20" s="55"/>
@@ -2095,28 +2158,28 @@
         <v>19</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C21" s="45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D21" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="80" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F21" s="47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G21" s="47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H21" s="47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I21" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J21" s="56"/>
       <c r="K21" s="56"/>
@@ -2127,33 +2190,33 @@
         <v>20</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E22" s="79" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F22" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="G22" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="G22" s="46" t="s">
-        <v>140</v>
-      </c>
       <c r="H22" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I22" s="55"/>
       <c r="J22" s="55"/>
       <c r="K22" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L22" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -2161,33 +2224,33 @@
         <v>21</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C23" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="46" t="s">
-        <v>62</v>
-      </c>
       <c r="E23" s="69" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F23" s="69" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G23" s="69" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H23" s="79" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I23" s="55"/>
       <c r="J23" s="55"/>
       <c r="K23" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L23" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -2195,33 +2258,33 @@
         <v>22</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" s="79" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F24" s="46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G24" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H24" s="46" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I24" s="55"/>
       <c r="J24" s="55"/>
       <c r="K24" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L24" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -2229,33 +2292,33 @@
         <v>23</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C25" s="45" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D25" s="45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E25" s="80" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G25" s="47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H25" s="47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I25" s="56"/>
       <c r="J25" s="56"/>
       <c r="K25" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L25" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -2266,19 +2329,19 @@
         <v>9</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E26" s="79"/>
       <c r="F26" s="46"/>
       <c r="G26" s="46"/>
       <c r="H26" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I26" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J26" s="55"/>
       <c r="K26" s="55"/>
@@ -2292,19 +2355,19 @@
         <v>9</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D27" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E27" s="80"/>
       <c r="F27" s="47"/>
       <c r="G27" s="47"/>
       <c r="H27" s="45" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I27" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J27" s="56"/>
       <c r="K27" s="56"/>
@@ -2318,24 +2381,24 @@
         <v>10</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E28" s="79"/>
       <c r="F28" s="46"/>
       <c r="G28" s="46"/>
       <c r="H28" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I28" s="55"/>
       <c r="J28" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K28" s="55"/>
       <c r="L28" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -2343,27 +2406,27 @@
         <v>27</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C29" s="45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E29" s="80"/>
       <c r="F29" s="47"/>
       <c r="G29" s="47"/>
       <c r="H29" s="45" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I29" s="56"/>
       <c r="J29" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K29" s="56"/>
       <c r="L29" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -2371,24 +2434,24 @@
         <v>28</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C30" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="E30" s="76"/>
       <c r="F30" s="50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G30" s="50"/>
       <c r="H30" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I30" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J30" s="57"/>
       <c r="K30" s="57"/>
@@ -2399,28 +2462,28 @@
         <v>29</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E31" s="79" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F31" s="46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G31" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H31" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I31" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J31" s="55"/>
       <c r="K31" s="55"/>
@@ -2431,28 +2494,28 @@
         <v>30</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C32" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D32" s="45" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E32" s="80" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F32" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G32" s="47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H32" s="47" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I32" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J32" s="56"/>
       <c r="K32" s="56"/>
@@ -2463,23 +2526,23 @@
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D33" s="51" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E33" s="86"/>
       <c r="F33" s="53"/>
       <c r="G33" s="53"/>
       <c r="H33" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I33" s="55"/>
       <c r="J33" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K33" s="55"/>
       <c r="L33" s="55"/>
@@ -2489,23 +2552,23 @@
         <v>32</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C34" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D34" s="52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E34" s="87"/>
       <c r="F34" s="54"/>
       <c r="G34" s="54"/>
       <c r="H34" s="45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I34" s="56"/>
       <c r="J34" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K34" s="56"/>
       <c r="L34" s="56"/>
@@ -2515,27 +2578,27 @@
         <v>33</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E35" s="79"/>
       <c r="F35" s="46"/>
       <c r="G35" s="46"/>
       <c r="H35" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I35" s="55"/>
       <c r="J35" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K35" s="55"/>
       <c r="L35" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -2543,27 +2606,27 @@
         <v>34</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C36" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D36" s="45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E36" s="80"/>
       <c r="F36" s="47"/>
       <c r="G36" s="47"/>
       <c r="H36" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I36" s="56"/>
       <c r="J36" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K36" s="56"/>
       <c r="L36" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -2571,28 +2634,28 @@
         <v>35</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C37" s="46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E37" s="79" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F37" s="46" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G37" s="46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H37" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I37" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J37" s="22"/>
       <c r="K37" s="22"/>
@@ -2603,28 +2666,28 @@
         <v>36</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D38" s="45" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E38" s="80" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F38" s="47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G38" s="47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H38" s="47" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I38" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J38" s="45"/>
       <c r="K38" s="45"/>
@@ -2635,28 +2698,28 @@
         <v>37</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C39" s="46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E39" s="86" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F39" s="53" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G39" s="53" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H39" s="53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I39" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J39" s="55"/>
       <c r="K39" s="55"/>
@@ -2667,28 +2730,28 @@
         <v>38</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C40" s="46" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E40" s="72" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F40" s="72" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G40" s="72" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H40" s="86" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I40" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J40" s="55"/>
       <c r="K40" s="55"/>
@@ -2699,25 +2762,25 @@
         <v>39</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>89</v>
+        <v>200</v>
       </c>
       <c r="D41" s="45" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E41" s="80" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F41" s="47"/>
       <c r="G41" s="47"/>
       <c r="H41" s="45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I41" s="56"/>
       <c r="J41" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K41" s="56"/>
       <c r="L41" s="56"/>
@@ -2733,7 +2796,7 @@
         <v>13</v>
       </c>
       <c r="D42" s="51" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E42" s="86"/>
       <c r="F42" s="53"/>
@@ -2744,10 +2807,10 @@
       <c r="I42" s="55"/>
       <c r="J42" s="55"/>
       <c r="K42" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L42" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
@@ -2761,7 +2824,7 @@
         <v>14</v>
       </c>
       <c r="D43" s="52" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E43" s="87"/>
       <c r="F43" s="54"/>
@@ -2772,10 +2835,10 @@
       <c r="I43" s="56"/>
       <c r="J43" s="56"/>
       <c r="K43" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L43" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
@@ -2786,28 +2849,28 @@
         <v>9</v>
       </c>
       <c r="C44" s="22" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D44" s="46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E44" s="79" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F44" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G44" s="46"/>
       <c r="H44" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I44" s="55"/>
       <c r="J44" s="55"/>
       <c r="K44" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L44" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
@@ -2818,28 +2881,28 @@
         <v>9</v>
       </c>
       <c r="C45" s="22" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D45" s="46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E45" s="68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F45" s="68" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G45" s="68"/>
       <c r="H45" s="71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I45" s="55"/>
       <c r="J45" s="55"/>
       <c r="K45" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L45" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
@@ -2850,28 +2913,28 @@
         <v>9</v>
       </c>
       <c r="C46" s="45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D46" s="47" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E46" s="78" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F46" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G46" s="45"/>
       <c r="H46" s="45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I46" s="45"/>
       <c r="J46" s="45"/>
       <c r="K46" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L46" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
@@ -2885,7 +2948,7 @@
         <v>15</v>
       </c>
       <c r="D47" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E47" s="84"/>
       <c r="F47" s="51"/>
@@ -2896,10 +2959,10 @@
       <c r="I47" s="55"/>
       <c r="J47" s="55"/>
       <c r="K47" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L47" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
@@ -2913,7 +2976,7 @@
         <v>16</v>
       </c>
       <c r="D48" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E48" s="84"/>
       <c r="F48" s="51"/>
@@ -2924,10 +2987,10 @@
       <c r="I48" s="55"/>
       <c r="J48" s="55"/>
       <c r="K48" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L48" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
@@ -2941,7 +3004,7 @@
         <v>17</v>
       </c>
       <c r="D49" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E49" s="84"/>
       <c r="F49" s="51"/>
@@ -2952,10 +3015,10 @@
       <c r="I49" s="55"/>
       <c r="J49" s="55"/>
       <c r="K49" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L49" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
@@ -2969,7 +3032,7 @@
         <v>18</v>
       </c>
       <c r="D50" s="52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E50" s="85"/>
       <c r="F50" s="52"/>
@@ -2980,10 +3043,10 @@
       <c r="I50" s="56"/>
       <c r="J50" s="56"/>
       <c r="K50" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L50" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
@@ -2991,27 +3054,27 @@
         <v>47</v>
       </c>
       <c r="B51" s="41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D51" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E51" s="84"/>
       <c r="F51" s="51"/>
       <c r="G51" s="51"/>
       <c r="H51" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I51" s="22"/>
       <c r="J51" s="22"/>
       <c r="K51" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L51" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
@@ -3019,27 +3082,27 @@
         <v>48</v>
       </c>
       <c r="B52" s="42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C52" s="45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D52" s="52" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E52" s="85"/>
       <c r="F52" s="52"/>
       <c r="G52" s="52"/>
       <c r="H52" s="45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I52" s="45"/>
       <c r="J52" s="45"/>
       <c r="K52" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L52" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
@@ -3050,26 +3113,26 @@
         <v>19</v>
       </c>
       <c r="C53" s="64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D53" s="73" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E53" s="71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F53" s="22"/>
       <c r="G53" s="22"/>
       <c r="H53" s="22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I53" s="55"/>
       <c r="J53" s="55"/>
       <c r="K53" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L53" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
@@ -3080,24 +3143,24 @@
         <v>20</v>
       </c>
       <c r="C54" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" s="52" t="s">
         <v>64</v>
-      </c>
-      <c r="D54" s="52" t="s">
-        <v>65</v>
       </c>
       <c r="E54" s="78"/>
       <c r="F54" s="45"/>
       <c r="G54" s="45"/>
       <c r="H54" s="45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I54" s="56"/>
       <c r="J54" s="56"/>
       <c r="K54" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L54" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
@@ -3105,27 +3168,27 @@
         <v>51</v>
       </c>
       <c r="B55" s="89" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C55" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55" s="64" t="s">
         <v>53</v>
-      </c>
-      <c r="D55" s="64" t="s">
-        <v>54</v>
       </c>
       <c r="E55" s="78"/>
       <c r="F55" s="45"/>
       <c r="G55" s="45"/>
       <c r="H55" s="50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I55" s="65"/>
       <c r="J55" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K55" s="65"/>
       <c r="L55" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
@@ -3133,26 +3196,26 @@
         <v>52</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D56" s="46" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E56" s="71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I56" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J56" s="55"/>
       <c r="K56" s="55"/>
@@ -3163,26 +3226,26 @@
         <v>53</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D57" s="46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E57" s="78" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F57" s="45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G57" s="45"/>
       <c r="H57" s="45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I57" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J57" s="55"/>
       <c r="K57" s="88"/>
@@ -3193,22 +3256,22 @@
         <v>54</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C58" s="46" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E58" s="71"/>
       <c r="F58" s="22"/>
       <c r="G58" s="22"/>
       <c r="H58" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I58" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J58" s="55"/>
       <c r="K58" s="55"/>
@@ -3222,19 +3285,19 @@
         <v>9</v>
       </c>
       <c r="C59" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D59" s="45" t="s">
         <v>51</v>
-      </c>
-      <c r="D59" s="45" t="s">
-        <v>52</v>
       </c>
       <c r="E59" s="78"/>
       <c r="F59" s="45"/>
       <c r="G59" s="45"/>
       <c r="H59" s="45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I59" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J59" s="56"/>
       <c r="K59" s="56"/>
@@ -3245,27 +3308,27 @@
         <v>56</v>
       </c>
       <c r="B60" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="D60" s="22" t="s">
         <v>92</v>
-      </c>
-      <c r="C60" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="D60" s="22" t="s">
-        <v>93</v>
       </c>
       <c r="E60" s="71"/>
       <c r="F60" s="22"/>
       <c r="G60" s="22"/>
       <c r="H60" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I60" s="55"/>
       <c r="J60" s="55"/>
       <c r="K60" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L60" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
@@ -3273,27 +3336,27 @@
         <v>57</v>
       </c>
       <c r="B61" s="44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C61" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D61" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E61" s="78"/>
       <c r="F61" s="45"/>
       <c r="G61" s="45"/>
       <c r="H61" s="45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I61" s="56"/>
       <c r="J61" s="56"/>
       <c r="K61" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L61" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="62" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -3304,19 +3367,19 @@
         <v>21</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E62" s="82"/>
       <c r="F62" s="64"/>
       <c r="G62" s="64"/>
       <c r="H62" s="64" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I62" s="65" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J62" s="65"/>
       <c r="K62" s="65"/>
@@ -3330,19 +3393,19 @@
         <v>22</v>
       </c>
       <c r="C63" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D63" s="45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E63" s="80"/>
       <c r="F63" s="47"/>
       <c r="G63" s="47"/>
       <c r="H63" s="47" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I63" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J63" s="56"/>
       <c r="K63" s="56"/>
@@ -3350,114 +3413,114 @@
     </row>
     <row r="64" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="67" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B64" s="35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C64" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D64" s="53" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E64" s="86"/>
       <c r="F64" s="53"/>
       <c r="G64" s="53"/>
       <c r="H64" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I64" s="46"/>
       <c r="J64" s="46"/>
       <c r="K64" s="55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L64" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C65" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D65" s="54" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E65" s="87"/>
       <c r="F65" s="54"/>
       <c r="G65" s="54"/>
       <c r="H65" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I65" s="56"/>
       <c r="J65" s="56"/>
       <c r="K65" s="56" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L65" s="60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B66" s="50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C66" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="C66" s="50" t="s">
+      <c r="D66" s="50" t="s">
         <v>124</v>
-      </c>
-      <c r="D66" s="50" t="s">
-        <v>125</v>
       </c>
       <c r="E66" s="76"/>
       <c r="F66" s="50"/>
       <c r="G66" s="50"/>
       <c r="H66" s="50" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I66" s="57"/>
       <c r="J66" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K66" s="57"/>
       <c r="L66" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B67" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C67" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="C67" s="50" t="s">
+      <c r="D67" s="50" t="s">
         <v>131</v>
-      </c>
-      <c r="D67" s="50" t="s">
-        <v>132</v>
       </c>
       <c r="E67" s="76"/>
       <c r="F67" s="50"/>
       <c r="G67" s="50"/>
       <c r="H67" s="50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I67" s="57"/>
       <c r="J67" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K67" s="57"/>
       <c r="L67" s="57" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.2">
@@ -3477,7 +3540,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="90" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
@@ -3546,10 +3609,10 @@
       <c r="I76" s="68"/>
     </row>
   </sheetData>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.23622047244094491" bottom="0.23622047244094491" header="3.937007874015748E-2" footer="3.937007874015748E-2"/>
-  <pageSetup paperSize="9" scale="52" orientation="landscape" cellComments="asDisplayed" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.39370078740157483" bottom="0.19685039370078741" header="0.19685039370078741" footer="3.937007874015748E-2"/>
+  <pageSetup paperSize="9" scale="51" orientation="landscape" cellComments="asDisplayed" horizontalDpi="0" verticalDpi="0"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri,Standard"&amp;K000000c’t-Bot Teensy 3.6 Pin Mapping</oddHeader>
+    <oddHeader>&amp;C&amp;"Calibri,Standard"&amp;16&amp;K000000c’t-Bot Teensy 3.6 Pin Mapping</oddHeader>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
mainboard: signal names updated
</commit_message>
<xml_diff>
--- a/teensy/teensy_3.6_pin_mapping.xlsx
+++ b/teensy/teensy_3.6_pin_mapping.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ts/src/ctbot/ct-bot-hw/teensy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BF8EEA9-8D11-354D-A961-72728FEE2E2B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4241A34-C5CA-2B48-8C45-AFBDDFB3922D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="40920" windowHeight="29060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="206">
   <si>
     <t>Pin</t>
   </si>
@@ -366,9 +366,6 @@
     <t>RPI_SCLK0</t>
   </si>
   <si>
-    <t>RPi SPI Slave SCKL</t>
-  </si>
-  <si>
     <t>RPI_SPI0_CE0</t>
   </si>
   <si>
@@ -585,9 +582,6 @@
     <t>I2C 2 (Ena, LED, LCD)</t>
   </si>
   <si>
-    <t>I2C 0 oder Uart</t>
-  </si>
-  <si>
     <t>A3/SDA0/PWM (TPM1)</t>
   </si>
   <si>
@@ -631,6 +625,27 @@
   </si>
   <si>
     <t>BAT_IN_FB</t>
+  </si>
+  <si>
+    <t>RX1</t>
+  </si>
+  <si>
+    <t>TX5</t>
+  </si>
+  <si>
+    <t>RX5</t>
+  </si>
+  <si>
+    <t>CS0</t>
+  </si>
+  <si>
+    <t>SCK0</t>
+  </si>
+  <si>
+    <t>RPi SPI Slave SCK</t>
+  </si>
+  <si>
+    <t>I2C 0 oder Uart 3</t>
   </si>
 </sst>
 </file>
@@ -1524,8 +1539,8 @@
   </sheetPr>
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1555,16 +1570,16 @@
         <v>85</v>
       </c>
       <c r="E1" s="75" t="s">
+        <v>147</v>
+      </c>
+      <c r="F1" s="62" t="s">
         <v>148</v>
       </c>
-      <c r="F1" s="62" t="s">
+      <c r="G1" s="62" t="s">
         <v>149</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="H1" s="62" t="s">
         <v>150</v>
-      </c>
-      <c r="H1" s="62" t="s">
-        <v>151</v>
       </c>
       <c r="I1" s="63" t="s">
         <v>54</v>
@@ -1636,22 +1651,22 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E4" s="76" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F4" s="50" t="s">
         <v>62</v>
       </c>
       <c r="G4" s="50" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H4" s="50" t="s">
         <v>9</v>
@@ -1670,13 +1685,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E5" s="71" t="s">
         <v>23</v>
@@ -1702,13 +1717,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="45" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="80" t="s">
         <v>24</v>
@@ -1734,10 +1749,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D7" s="46" t="s">
         <v>23</v>
@@ -1746,10 +1761,10 @@
         <v>35</v>
       </c>
       <c r="F7" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G7" s="46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H7" s="46" t="s">
         <v>23</v>
@@ -1766,7 +1781,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C8" s="47" t="s">
         <v>34</v>
@@ -1778,10 +1793,10 @@
         <v>61</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G8" s="47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H8" s="47" t="s">
         <v>24</v>
@@ -1800,25 +1815,25 @@
         <v>7</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="E9" s="79" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G9" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H9" s="46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I9" s="55"/>
       <c r="J9" s="55"/>
@@ -1834,25 +1849,25 @@
         <v>8</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="E10" s="81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F10" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G10" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H10" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I10" s="58"/>
       <c r="J10" s="58"/>
@@ -1868,10 +1883,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D11" s="22" t="s">
         <v>107</v>
@@ -1880,7 +1895,7 @@
       <c r="F11" s="46"/>
       <c r="G11" s="46"/>
       <c r="H11" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I11" s="55" t="s">
         <v>56</v>
@@ -1896,10 +1911,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" s="49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="49" t="s">
         <v>108</v>
@@ -1908,7 +1923,7 @@
       <c r="F12" s="48"/>
       <c r="G12" s="48"/>
       <c r="H12" s="49" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I12" s="58" t="s">
         <v>56</v>
@@ -1927,7 +1942,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="D13" s="22" t="s">
         <v>104</v>
@@ -1955,7 +1970,7 @@
         <v>7</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="D14" s="45" t="s">
         <v>105</v>
@@ -2006,13 +2021,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>111</v>
+        <v>203</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>112</v>
+        <v>204</v>
       </c>
       <c r="E16" s="79"/>
       <c r="F16" s="46"/>
@@ -2034,10 +2049,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C17" s="45" t="s">
-        <v>113</v>
+        <v>202</v>
       </c>
       <c r="D17" s="45" t="s">
         <v>106</v>
@@ -2046,7 +2061,7 @@
       <c r="F17" s="47"/>
       <c r="G17" s="47"/>
       <c r="H17" s="45" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="I17" s="56"/>
       <c r="J17" s="56" t="s">
@@ -2062,10 +2077,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C18" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D18" s="22" t="s">
         <v>40</v>
@@ -2074,13 +2089,13 @@
         <v>27</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G18" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H18" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I18" s="55" t="s">
         <v>56</v>
@@ -2094,10 +2109,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>41</v>
@@ -2106,13 +2121,13 @@
         <v>28</v>
       </c>
       <c r="F19" s="69" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G19" s="69" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H19" s="79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I19" s="55" t="s">
         <v>56</v>
@@ -2135,7 +2150,7 @@
         <v>42</v>
       </c>
       <c r="E20" s="79" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F20" s="46" t="s">
         <v>25</v>
@@ -2167,7 +2182,7 @@
         <v>43</v>
       </c>
       <c r="E21" s="80" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F21" s="47" t="s">
         <v>26</v>
@@ -2190,7 +2205,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>59</v>
@@ -2202,10 +2217,10 @@
         <v>25</v>
       </c>
       <c r="F22" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="G22" s="46" t="s">
         <v>138</v>
-      </c>
-      <c r="G22" s="46" t="s">
-        <v>139</v>
       </c>
       <c r="H22" s="46" t="s">
         <v>35</v>
@@ -2224,7 +2239,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>60</v>
@@ -2236,10 +2251,10 @@
         <v>26</v>
       </c>
       <c r="F23" s="69" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G23" s="69" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H23" s="79" t="s">
         <v>61</v>
@@ -2258,7 +2273,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>65</v>
@@ -2267,13 +2282,13 @@
         <v>62</v>
       </c>
       <c r="E24" s="79" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F24" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G24" s="46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H24" s="46" t="s">
         <v>62</v>
@@ -2292,25 +2307,25 @@
         <v>23</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C25" s="45" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D25" s="45" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E25" s="80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F25" s="47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G25" s="47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H25" s="47" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I25" s="56"/>
       <c r="J25" s="56"/>
@@ -2381,7 +2396,7 @@
         <v>10</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="D28" s="22" t="s">
         <v>29</v>
@@ -2409,7 +2424,7 @@
         <v>73</v>
       </c>
       <c r="C29" s="45" t="s">
-        <v>31</v>
+        <v>199</v>
       </c>
       <c r="D29" s="45" t="s">
         <v>29</v>
@@ -2462,13 +2477,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C31" s="22" t="s">
         <v>99</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E31" s="79" t="s">
         <v>62</v>
@@ -2480,7 +2495,7 @@
         <v>35</v>
       </c>
       <c r="H31" s="46" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I31" s="55" t="s">
         <v>56</v>
@@ -2494,16 +2509,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C32" s="45" t="s">
         <v>100</v>
       </c>
       <c r="D32" s="45" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E32" s="80" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F32" s="47" t="s">
         <v>24</v>
@@ -2512,7 +2527,7 @@
         <v>61</v>
       </c>
       <c r="H32" s="47" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I32" s="56" t="s">
         <v>56</v>
@@ -2526,7 +2541,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C33" s="22" t="s">
         <v>36</v>
@@ -2552,7 +2567,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C34" s="45" t="s">
         <v>37</v>
@@ -2578,10 +2593,10 @@
         <v>33</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>95</v>
+        <v>200</v>
       </c>
       <c r="D35" s="22" t="s">
         <v>87</v>
@@ -2606,10 +2621,10 @@
         <v>34</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C36" s="45" t="s">
-        <v>96</v>
+        <v>201</v>
       </c>
       <c r="D36" s="45" t="s">
         <v>87</v>
@@ -2634,25 +2649,25 @@
         <v>35</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C37" s="46" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D37" s="22" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E37" s="79" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F37" s="46" t="s">
         <v>35</v>
       </c>
       <c r="G37" s="46" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H37" s="46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I37" s="55" t="s">
         <v>56</v>
@@ -2666,25 +2681,25 @@
         <v>36</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C38" s="47" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D38" s="45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E38" s="80" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F38" s="47" t="s">
         <v>61</v>
       </c>
       <c r="G38" s="47" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H38" s="47" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I38" s="56" t="s">
         <v>56</v>
@@ -2698,25 +2713,25 @@
         <v>37</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C39" s="46" t="s">
         <v>27</v>
       </c>
       <c r="D39" s="22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E39" s="86" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F39" s="53" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G39" s="53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H39" s="53" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I39" s="55" t="s">
         <v>56</v>
@@ -2730,25 +2745,25 @@
         <v>38</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C40" s="46" t="s">
         <v>28</v>
       </c>
       <c r="D40" s="22" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E40" s="72" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F40" s="72" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G40" s="72" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H40" s="86" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I40" s="55" t="s">
         <v>56</v>
@@ -2765,7 +2780,7 @@
         <v>75</v>
       </c>
       <c r="C41" s="45" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D41" s="45" t="s">
         <v>66</v>
@@ -2852,17 +2867,17 @@
         <v>80</v>
       </c>
       <c r="D44" s="46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E44" s="79" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F44" s="46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G44" s="46"/>
       <c r="H44" s="46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I44" s="55"/>
       <c r="J44" s="55"/>
@@ -2884,7 +2899,7 @@
         <v>81</v>
       </c>
       <c r="D45" s="46" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E45" s="68" t="s">
         <v>50</v>
@@ -2916,7 +2931,7 @@
         <v>82</v>
       </c>
       <c r="D46" s="47" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E46" s="78" t="s">
         <v>48</v>
@@ -2926,7 +2941,7 @@
       </c>
       <c r="G46" s="45"/>
       <c r="H46" s="45" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I46" s="45"/>
       <c r="J46" s="45"/>
@@ -3168,7 +3183,7 @@
         <v>51</v>
       </c>
       <c r="B55" s="89" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C55" s="64" t="s">
         <v>52</v>
@@ -3196,23 +3211,23 @@
         <v>52</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D56" s="46" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E56" s="71" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F56" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G56" s="22"/>
       <c r="H56" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I56" s="55" t="s">
         <v>56</v>
@@ -3226,23 +3241,23 @@
         <v>53</v>
       </c>
       <c r="B57" s="37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C57" s="22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D57" s="46" t="s">
         <v>86</v>
       </c>
       <c r="E57" s="78" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F57" s="45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G57" s="45"/>
       <c r="H57" s="45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I57" s="55" t="s">
         <v>56</v>
@@ -3256,13 +3271,13 @@
         <v>54</v>
       </c>
       <c r="B58" s="37" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C58" s="46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E58" s="71"/>
       <c r="F58" s="22"/>
@@ -3367,7 +3382,7 @@
         <v>21</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D62" s="22" t="s">
         <v>38</v>
@@ -3393,7 +3408,7 @@
         <v>22</v>
       </c>
       <c r="C63" s="45" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D63" s="45" t="s">
         <v>39</v>
@@ -3413,10 +3428,10 @@
     </row>
     <row r="64" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="67" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B64" s="35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C64" s="46" t="s">
         <v>101</v>
@@ -3441,10 +3456,10 @@
     </row>
     <row r="65" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C65" s="47" t="s">
         <v>102</v>
@@ -3469,22 +3484,22 @@
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B66" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="C66" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="C66" s="50" t="s">
+      <c r="D66" s="50" t="s">
         <v>123</v>
-      </c>
-      <c r="D66" s="50" t="s">
-        <v>124</v>
       </c>
       <c r="E66" s="76"/>
       <c r="F66" s="50"/>
       <c r="G66" s="50"/>
       <c r="H66" s="50" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I66" s="57"/>
       <c r="J66" s="57" t="s">
@@ -3497,22 +3512,22 @@
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B67" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="C67" s="50" t="s">
+      <c r="D67" s="50" t="s">
         <v>130</v>
-      </c>
-      <c r="D67" s="50" t="s">
-        <v>131</v>
       </c>
       <c r="E67" s="76"/>
       <c r="F67" s="50"/>
       <c r="G67" s="50"/>
       <c r="H67" s="50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="I67" s="57"/>
       <c r="J67" s="57" t="s">
@@ -3540,7 +3555,7 @@
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71" s="90" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>

</xml_diff>